<commit_message>
final design, final code, test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eileen Martinez\PycharmProjects\cs151-pa1-ajduenomartinez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52CCF8-20CB-4865-9671-DC5A47E6791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="8180" yWindow="0" windowWidth="14470" windowHeight="15130" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,23 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>You need to create your own tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              Intro segment:                                                              </t>
   </si>
 </sst>
 </file>
@@ -391,15 +385,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,6 +402,11 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
final design, code, test cases and reflection
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eileen Martinez\PycharmProjects\cs151-pa1-ajduenomartinez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F52CCF8-20CB-4865-9671-DC5A47E6791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A52736A-3FAB-4E0C-951F-6356510A5B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="0" windowWidth="14470" windowHeight="15130" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="15130" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,12 +25,219 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>You need to create your own tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                              Intro segment:                                                              </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Prompt 1:</t>
+  </si>
+  <si>
+    <t>DATA IN:</t>
+  </si>
+  <si>
+    <t>DATA OUT:</t>
+  </si>
+  <si>
+    <t>Valid name</t>
+  </si>
+  <si>
+    <t>Invalid name, enter valid name</t>
+  </si>
+  <si>
+    <t>prompt 2:</t>
+  </si>
+  <si>
+    <t>stay or leave elevator?</t>
+  </si>
+  <si>
+    <t>Proceed to next prompt</t>
+  </si>
+  <si>
+    <t>output ending 1, program ends</t>
+  </si>
+  <si>
+    <t>invalid input, enter valid input</t>
+  </si>
+  <si>
+    <t>prompt 3:</t>
+  </si>
+  <si>
+    <t>What floor?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ""</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>proceed to story option 1</t>
+  </si>
+  <si>
+    <t>proceed to story option 2</t>
+  </si>
+  <si>
+    <t>proceed to story option 3</t>
+  </si>
+  <si>
+    <t>prompt 4:</t>
+  </si>
+  <si>
+    <t>speak to mole?</t>
+  </si>
+  <si>
+    <t>mole dialogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other dialogue </t>
+  </si>
+  <si>
+    <t>Prompt 5:</t>
+  </si>
+  <si>
+    <t>go to mines or inn?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"" </t>
+  </si>
+  <si>
+    <t>proceed to prompt 7</t>
+  </si>
+  <si>
+    <t>proceed to prompt 6</t>
+  </si>
+  <si>
+    <t>prompt 6</t>
+  </si>
+  <si>
+    <t>stay or leave inn?</t>
+  </si>
+  <si>
+    <t>output ending 2, end program</t>
+  </si>
+  <si>
+    <t>prompt 7:</t>
+  </si>
+  <si>
+    <t>what path in mines?</t>
+  </si>
+  <si>
+    <t>output path 1 dialogue</t>
+  </si>
+  <si>
+    <t>output path 2 dialogue</t>
+  </si>
+  <si>
+    <t>break loop, output ending 3, end program</t>
+  </si>
+  <si>
+    <t>prompt 8:</t>
+  </si>
+  <si>
+    <t>cross river or bridge:</t>
+  </si>
+  <si>
+    <t>output ending 4, end program</t>
+  </si>
+  <si>
+    <t>proceed to prompt 9</t>
+  </si>
+  <si>
+    <t>prompt 9</t>
+  </si>
+  <si>
+    <t>how much money to give gnome?</t>
+  </si>
+  <si>
+    <t>Gnome is upset, proceed to prompt 10</t>
+  </si>
+  <si>
+    <t>gnome allows user to proceed to prompt 10</t>
+  </si>
+  <si>
+    <t>gnome happily lets user proceed proceed to prompt 10</t>
+  </si>
+  <si>
+    <t>gnome jumps for joy. proceed to prompt 10</t>
+  </si>
+  <si>
+    <t>gnome passes out. proceed to prompt 10</t>
+  </si>
+  <si>
+    <t>prompt 10</t>
+  </si>
+  <si>
+    <t>go to witches hut?</t>
+  </si>
+  <si>
+    <t>proceed to prompt 11</t>
+  </si>
+  <si>
+    <t>output ending 5, end program</t>
+  </si>
+  <si>
+    <t>prompt 11</t>
+  </si>
+  <si>
+    <t>sleep or drink fairy fountain?</t>
+  </si>
+  <si>
+    <t>output ending 7, end program</t>
+  </si>
+  <si>
+    <t>output ending 8, end program</t>
+  </si>
+  <si>
+    <t>prompt 12</t>
+  </si>
+  <si>
+    <t>go to next room or go to bathroom</t>
+  </si>
+  <si>
+    <t>proceed to prompt 13</t>
+  </si>
+  <si>
+    <t>prompt 13</t>
+  </si>
+  <si>
+    <t>stay or leave bathroom</t>
+  </si>
+  <si>
+    <t>proceed to prompt 14</t>
+  </si>
+  <si>
+    <t>prompt 14</t>
+  </si>
+  <si>
+    <t>left door or right door?</t>
+  </si>
+  <si>
+    <t>proceed to prompt 15</t>
+  </si>
+  <si>
+    <t>output break room dialogue, proceed to prompt 15</t>
+  </si>
+  <si>
+    <t>prompt 15</t>
+  </si>
+  <si>
+    <t>up stairs or down stairs?</t>
+  </si>
+  <si>
+    <t>output ending 6, end program.</t>
+  </si>
+  <si>
+    <t>output ending 9, end program</t>
+  </si>
+  <si>
+    <t>program check:</t>
+  </si>
+  <si>
+    <t>proceed to endings 10 and 11, end program</t>
   </si>
 </sst>
 </file>
@@ -66,11 +273,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,32 +589,701 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>0.12</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>2.34</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>7.23</v>
+      </c>
+      <c r="C69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="C70" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>14.32</v>
+      </c>
+      <c r="C71" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>17.78</v>
+      </c>
+      <c r="C72" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>21.67</v>
+      </c>
+      <c r="C73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>